<commit_message>
adding in alejandro's change because I couldn't fix the merge between .xlsx
</commit_message>
<xml_diff>
--- a/Terminators/Terminators.xlsx
+++ b/Terminators/Terminators.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vinoo/_dev/distribution/iGEM-distribution/Terminators/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79163C59-D5B2-3B4A-9CD9-A87DF615B76D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFB8A452-BF0B-CA47-B8F2-FE4EE0464A8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-30880" yWindow="-1560" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7634" uniqueCount="7560">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7639" uniqueCount="7563">
   <si>
     <t>Collection Name</t>
   </si>
@@ -22783,6 +22783,15 @@
   </si>
   <si>
     <t>BBa_B0015, BBa_B0010, BBa_B0012, BBa_B1006_T_U10, rnpB_T1, rpoC_T</t>
+  </si>
+  <si>
+    <t>STOP_MC</t>
+  </si>
+  <si>
+    <t>AA</t>
+  </si>
+  <si>
+    <t>To make the stop codon when placed after CDS_TT_OH</t>
   </si>
 </sst>
 </file>
@@ -23654,8 +23663,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M983"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -24301,9 +24310,15 @@
       <c r="M23" s="18"/>
     </row>
     <row r="24" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A24" s="18"/>
-      <c r="B24" s="18"/>
-      <c r="C24" s="18"/>
+      <c r="A24" s="18" t="s">
+        <v>7560</v>
+      </c>
+      <c r="B24" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="C24" s="18" t="s">
+        <v>7562</v>
+      </c>
       <c r="D24" s="21"/>
       <c r="E24" s="18"/>
       <c r="F24" s="18"/>
@@ -24318,9 +24333,11 @@
       </c>
       <c r="L24" s="15">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M24" s="18"/>
+        <v>2</v>
+      </c>
+      <c r="M24" s="18" t="s">
+        <v>7561</v>
+      </c>
     </row>
     <row r="25" spans="1:13" ht="15.75" customHeight="1">
       <c r="A25" s="18"/>
@@ -25628,7 +25645,7 @@
   <dimension ref="A1:Z20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H34" sqref="H34"/>
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -26135,13 +26152,15 @@
       <c r="G14" s="22" t="s">
         <v>7555</v>
       </c>
-      <c r="H14" s="18" t="s">
+      <c r="H14" t="s">
+        <v>7560</v>
+      </c>
+      <c r="I14" s="18" t="s">
         <v>7559</v>
       </c>
-      <c r="I14" s="34" t="s">
+      <c r="J14" s="34" t="s">
         <v>7556</v>
       </c>
-      <c r="J14" s="18"/>
       <c r="K14" s="18"/>
       <c r="L14" s="18"/>
       <c r="M14" s="18"/>

</xml_diff>